<commit_message>
Small changes have been added like Google Analytics tag , changes of <title> , <meta> and some content sizes
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mamadou\Desktop\Développement Web\Parcours Développeur Web Openclassrooms\Livrables\P4_Dembele Mamadou\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86F5896-0C01-44E9-B30C-D4B71662CABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39BCCDD-150C-454F-9CCB-7DD745ED79FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,17 +51,155 @@
     <t>Référence</t>
   </si>
   <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-title/</t>
+  </si>
+  <si>
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Vitesse du site</t>
+    <t>Couleurs Arrières Plan</t>
+  </si>
+  <si>
+    <t>Elle ne sont pas suffisamment contrastées</t>
+  </si>
+  <si>
+    <t>Ajuster les couleurs de manière à mettre en valeur le contenu de la page</t>
+  </si>
+  <si>
+    <t>https://colorable.jxnblk.com/ffffff/000000</t>
+  </si>
+  <si>
+    <t>Performances</t>
+  </si>
+  <si>
+    <t>Poids des images</t>
+  </si>
+  <si>
+    <t>Elles ont un impact sur le chargement de la page impactant ainsi son poids</t>
+  </si>
+  <si>
+    <t>Compresser les images</t>
+  </si>
+  <si>
+    <t>Utiliser un outil de compression d'images</t>
+  </si>
+  <si>
+    <t>https://imagecompressor.com/fr/</t>
+  </si>
+  <si>
+    <t>Formats des images</t>
+  </si>
+  <si>
+    <t>Faible compression des images</t>
+  </si>
+  <si>
+    <t>Convertir les images au formats WebP ou AVIF</t>
+  </si>
+  <si>
+    <t>Utiliser un outil de conversion d'images</t>
+  </si>
+  <si>
+    <t>https://convertio.co/fr/png-webp/</t>
+  </si>
+  <si>
+    <t>Il est court et non explicite</t>
+  </si>
+  <si>
+    <t>Indiquer le nom de l'agence ainsi que son activité</t>
+  </si>
+  <si>
+    <t>La description du site</t>
+  </si>
+  <si>
+    <t>Le titre de l'onglet du site</t>
+  </si>
+  <si>
+    <t>Cette dernière est vide dans le code source</t>
+  </si>
+  <si>
+    <t>Profiter des 165 caractères de la balise &lt;meta&gt; pour la description</t>
+  </si>
+  <si>
+    <t>Profiter des 65 caractères proposés par la balise &lt;title&gt; pour les résultats de recherches</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
+  </si>
+  <si>
+    <t>Insérer des mots clés relatant l'activité de l'entreprise</t>
+  </si>
+  <si>
+    <t>Google Analytics</t>
+  </si>
+  <si>
+    <t>Aucune intégration de Google Analytics</t>
+  </si>
+  <si>
+    <t>Utiliser cet outil pour analyser et optimiser l'expérience utilisateur</t>
+  </si>
+  <si>
+    <t>Implémenter l'outil directement dans le code source</t>
+  </si>
+  <si>
+    <t>https://marketingplatform.google.com/intl/fr/about/analytics/</t>
+  </si>
+  <si>
+    <t>Polices d'écriture</t>
+  </si>
+  <si>
+    <t>Changer la taille des polices</t>
+  </si>
+  <si>
+    <t>La taille des polices sur bureau et version mobile notamment pour la page d'accueil ne sont pas assez grandes</t>
+  </si>
+  <si>
+    <t>https://chrome.google.com/webstore/detail/lighthouse/blipmdconlkpinefehnmjammfjpmpbjk?hl=fr</t>
+  </si>
+  <si>
+    <t>Augmenter la taille de la police selon le support</t>
+  </si>
+  <si>
+    <t>Taille du site</t>
+  </si>
+  <si>
+    <t>La taille du site est impactée notamment en terme de ressources que ce soit pour les polices ou les librairies utilisées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire l'impact des ressources </t>
+  </si>
+  <si>
+    <t>https://www.imagescreations.fr/qu-est-ce-qu-un-cdn-quel-interet-en-seo-et-pour-votre-site-web/</t>
+  </si>
+  <si>
+    <t>Chargement de la page</t>
+  </si>
+  <si>
+    <t>Les espaces non utilisées notamment dans les fichiers css et javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer tout ce qui est espace inutile afin d'augmenter le chargement de la page </t>
+  </si>
+  <si>
+    <t>Utiliser un outil pour minifier les fichiers CSS et JS</t>
+  </si>
+  <si>
+    <t>https://www.websiteplanet.com/fr/webtools/jscssminifier/</t>
+  </si>
+  <si>
+    <t>Utiliser colorable qui permet d'adapter les options d'une couleur vis à du Web Content Accessibility Guidelines</t>
+  </si>
+  <si>
+    <t>Dans la mesure du possible utiliser des CDN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,13 +221,37 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -107,14 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -123,19 +278,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,125 +539,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="26" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="107.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" style="13" customWidth="1"/>
+    <col min="27" max="16384" width="11.33203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="14" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4"/>
+    <row r="8" spans="1:26" s="14" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
+    <row r="10" spans="1:26" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="4"/>
+    <row r="11" spans="1:26" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="4"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="4"/>
+      <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1435,9 +1806,18 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{17AEE622-4F20-4C02-A0F2-208674D90061}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{7FB25A2E-6602-420D-9137-B3B0F48CB5BA}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{2367944F-4185-48CD-B0A7-55AF9A9C0B01}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{63A42E4A-6D42-454B-AD3A-29B5583499FF}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{A48CB0C4-8318-4771-85D5-478DBD91CC77}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{95054326-1952-4A0A-85A5-C60F44ED80A6}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{B98D0D72-D4AC-47B1-A697-164CF28ADE36}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{885F461D-3C81-4F34-9A3D-4225F4C5B7C2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>